<commit_message>
Running additional workloads D, E and F, to expand further the comparative analysis using YCSB for MySQL, Cassandra, and MongoDB completed.
</commit_message>
<xml_diff>
--- a/YCSB_Summary_Outputs.xlsx
+++ b/YCSB_Summary_Outputs.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydbs-my.sharepoint.com/personal/10539218_mydbs_ie/Documents/Desktop/CA2_Integrated_Assesment_MSc_Data_Analytics_CCT_Semester_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="270" documentId="8_{5797AAB6-4CD0-4188-962D-1F53B339BC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E73CCC45-8C51-43E7-8640-E8274BC54ACD}"/>
+  <xr:revisionPtr revIDLastSave="280" documentId="8_{5797AAB6-4CD0-4188-962D-1F53B339BC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF7C2D36-2686-4539-BCA8-EB99F88B9EBB}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="23640" activeTab="2" xr2:uid="{48F0A246-731E-42DF-AEB8-358F28B279A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{48F0A246-731E-42DF-AEB8-358F28B279A1}"/>
   </bookViews>
   <sheets>
     <sheet name="MySQL" sheetId="1" r:id="rId1"/>
     <sheet name="MongoDB" sheetId="2" r:id="rId2"/>
     <sheet name="Cassandra" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="32">
   <si>
     <t>READ</t>
   </si>
@@ -80,6 +81,60 @@
   </si>
   <si>
     <t>Workload G</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Read/Write</t>
+  </si>
+  <si>
+    <t>Latency/Durability</t>
+  </si>
+  <si>
+    <t>Sync/Async</t>
+  </si>
+  <si>
+    <t>Row/Column optimized</t>
+  </si>
+  <si>
+    <t>Replication</t>
+  </si>
+  <si>
+    <t>Durability</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Sync</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Cassandra</t>
+  </si>
+  <si>
+    <t>Tunable</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>Master-Slave</t>
+  </si>
+  <si>
+    <t>MongoDB</t>
+  </si>
+  <si>
+    <t>Document (Row)</t>
+  </si>
+  <si>
+    <t>Replica Set</t>
   </si>
 </sst>
 </file>
@@ -121,10 +176,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,7 +558,7 @@
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1267,7 +1321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5E162C-4776-4AFE-9EF3-D2EB298C8502}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -1661,4 +1715,107 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D03E1D-E559-40A1-9CE2-4B694AD61BB7}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>